<commit_message>
3469: Fixed failing specs, allowed underscore
</commit_message>
<xml_diff>
--- a/spec/fixtures/user_batches/email_problems.xlsx
+++ b/spec/fixtures/user_batches/email_problems.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Full Name</t>
   </si>
@@ -70,13 +70,31 @@
   </si>
   <si>
     <t>+9837494434</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>eee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +129,14 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -145,6 +171,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,101 +504,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>